<commit_message>
Updates 12S and 16S taxa tables, databases, and outputs from DADA2 to include notes from NCBI BLAST and increased taxa.
</commit_message>
<xml_diff>
--- a/DADA2/WADE003-arcticpred-12SP1-taxa-130trunc.xlsx
+++ b/DADA2/WADE003-arcticpred-12SP1-taxa-130trunc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intern\Arctic-predator-diet-microbiome\DADA2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/DADA2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="279" documentId="11_CD0A024B572A2E808DD41CFD5F350142668DA2EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{521FA630-931C-4A9C-9287-9472D9259F7D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="505">
   <si>
     <t>rownames</t>
   </si>
@@ -1192,13 +1193,355 @@
   </si>
   <si>
     <t xml:space="preserve">100% matches: Glyptocephalus stelleri, Glyptocephalus zachirus, Myzopsetta proboscidea, </t>
+  </si>
+  <si>
+    <t>no 100% match: 98.72% Spirinchus thaleichthys</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Elenginus gracilis</t>
+  </si>
+  <si>
+    <t>100% matches: Gymnocanthus intermedius, Gymnocanthus pistilliger</t>
+  </si>
+  <si>
+    <t>100% matches: Liparis gibbus, Liparis ochotensis</t>
+  </si>
+  <si>
+    <t>100% matches: Lumpenus fabricii, Leptoclinus maculatus</t>
+  </si>
+  <si>
+    <t>Gymnocanthus tricuspis</t>
+  </si>
+  <si>
+    <t>no 100% matches: 99.36% Myoxocephalus scorpius, Myoxocephalus quadricornis, Myoxocephalus thompsonii, Myoxocephalus aenaeus</t>
+  </si>
+  <si>
+    <t>no 100% matches: 99.36% Osmerus mordax dentex</t>
+  </si>
+  <si>
+    <t>no 100% matches: 99.36% Myoxocephalus stelleri, Myoxocephalus jaok, Myoxocephalus polyacanthocephalus</t>
+  </si>
+  <si>
+    <t>100% matches: Hemilepidotus papilio, Hemilepidotus jordani</t>
+  </si>
+  <si>
+    <t>100% matches :Myoxocephalus stelleri, Myoxocephalus jaok, Myoxocephalus polyacanthocephalu</t>
+  </si>
+  <si>
+    <t>no 100% matches: 99.36% Hypomesus olidus</t>
+  </si>
+  <si>
+    <t>Boreogadus saida</t>
+  </si>
+  <si>
+    <t>no 100% matches:  99.36% Osmerus mordax dentex</t>
+  </si>
+  <si>
+    <t>100% matches: Lepidopsetta polyxystra, Lepidopsetta bilineata</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Eleginus gracilis</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Osmerus mordax dentex</t>
+  </si>
+  <si>
+    <t>no 100% match: 94.08% Sagmatias obliquidens</t>
+  </si>
+  <si>
+    <t>Liparis tunicatus</t>
+  </si>
+  <si>
+    <t>Stichaeus punctatus</t>
+  </si>
+  <si>
+    <t>100% matches: Pleuronectes quadrituberculatus, Pleuronectes platessa</t>
+  </si>
+  <si>
+    <t>no 100% matches:  94.08% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no 100% match: 99.36% Hypomesus olidus </t>
+  </si>
+  <si>
+    <t>no 100% match: 99.73% Microgadus tomcod</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Eurymen gyrinus</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Lumpenus fabricii, Leptoclinus maculatus</t>
+  </si>
+  <si>
+    <t>Nautichthys pribilovius</t>
+  </si>
+  <si>
+    <t>NO SIGNIFICANT MATCH</t>
+  </si>
+  <si>
+    <t>no 100% match: 97.44% Pusa hispida</t>
+  </si>
+  <si>
+    <t>Acantholumpenus mackayi</t>
+  </si>
+  <si>
+    <t>no 100% match: 93.12% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>100% matches: Podothecus veternus, Sarritor frenatus, Leptagonus decagonus</t>
+  </si>
+  <si>
+    <t>100% matches: Hippoglossoides robustus, Limanda limanda, Limanda aspera, Hippoglossoides elassodon, Limanda sakhalinensis, Hippoglossoides platessoides, Pseudopleuronectes americanus, Hippoglossoides dubius, Cleisthenes pinetorum, Cleisthenes herzensteini</t>
+  </si>
+  <si>
+    <t>no 100% match: 88.82 Mesoplodon grayi</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.73% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 91.77% Delphinapterus leucas, Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Glyptocephalus stelleri, Glyptocephalus zachirus, Myzopsetta proboscidea</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Platichthys stellatus, Platichthys flesus, Myzopsetta ferruginea, Kareius bicoloratus x Platichthys stellatu (hybrid), Liopsetta glacialis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% matches: Coregonus lavaretus, Coregonus macrophthalmus, Coregonus oxyrinchus, Coregonus baicalensis, Coregonus clupeaformis, Coregonus migratorius, Coregonus maraena, Coregonus muksu, Coregonus ussuriensis, Coregonus peled, Coregonus steinmanni, Coregonus cluncaformis, Coregonus nasus </t>
+  </si>
+  <si>
+    <t>no 100% match: 99.65% Osmerus mordax dentex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no 100% match: 99.36% Glyptocephalus zachirus, Limanda limanda, Limanda sakhalinensis, Hippoglossoides elassodon, Hippoglossoides dubius, Limanda aspera, Hippoglossoides platessoides, Hippoglossoides robustus, Cleisthenes pinetorum, Myzopsetta proboscidea, Cleisthenes herzensteini, Hippoglossoides platessoides, Pseudopleuronectes americanus, Glyptocephalus zachirus, </t>
+  </si>
+  <si>
+    <t>100% matches: Liparis gibbus, Liparis ochotensis, Liparis ochotensis, Liparis bathyarcticus</t>
+  </si>
+  <si>
+    <t>no 100% match: 95.35% Mesoplodon densirostris</t>
+  </si>
+  <si>
+    <t>no 100% match: 97.10% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.32% Osmerus mordax dentex</t>
+  </si>
+  <si>
+    <t>no 100% match: 95% Orcaella heinsohni</t>
+  </si>
+  <si>
+    <t>no 100% match: 98.08% Pungitius pungitius, Pungitius laevis</t>
+  </si>
+  <si>
+    <t>no 100% match: 98.08% Gasterosteus aculeatus, Gasterosteus nipponicus</t>
+  </si>
+  <si>
+    <t>no 100% match: 88.61% Mesoplodon densirostris</t>
+  </si>
+  <si>
+    <t>100% match: "Uncultured bacertium,"Clostridium moniliforme, Eubacterium moniliforme)</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Oncorhynchus gorbuscha</t>
+  </si>
+  <si>
+    <t>no 100% match: 98.73% Microcottus sellaris</t>
+  </si>
+  <si>
+    <t>no 100% match: 96.79% Pusa hispida, Pusa siberica</t>
+  </si>
+  <si>
+    <t>no 100% match: 96.20% Delphinapterus leucas, Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 95.50% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 85.35% Mesoplodon densirostris</t>
+  </si>
+  <si>
+    <t>Oncorhynchus gorbuscha</t>
+  </si>
+  <si>
+    <t>no 100% match: 86.16% Indopacetus pacificus</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Oncorhynchus kisutch</t>
+  </si>
+  <si>
+    <t>100% matches: Clostridium fallax, "Uncultured bacterium"</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Ammodytes hexapterus</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Gadus chalcogrammus, Gadus morhua</t>
+  </si>
+  <si>
+    <t>no 100% match (no matches that made sense either)</t>
+  </si>
+  <si>
+    <t>no 100% match: 98.10% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.08% Eleginus gracilis</t>
+  </si>
+  <si>
+    <t>no 100% match: 98.73% Eleginus gracilis</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.05% Eleginus gracilis</t>
+  </si>
+  <si>
+    <t>no 100% match: 97.47% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 96.82% Myoxocephalus brandtii, Myoxocephalus quadricornis, Myoxocephalus aenaeus, Myoxocephalus scorpius, Myoxocephalus thompsonii</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.38% Mallotus villosus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no 100% match (no matches that made sense) </t>
+  </si>
+  <si>
+    <t>no 100% match: 88.61% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match: 94.94% Delphinapterus leucas, Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 89.24% Mesoplodon densirostris</t>
+  </si>
+  <si>
+    <t>no 100% match: 90.75% Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.37% Coregonus lavaretus, Coregonus macrophthalmus, Coregonus oxyrinchus, Coregonus baicalensis, Coregonus clupeaformis, Coregonus migratorius, Coregonus zugerbalchen, Coregonus maraena, Coregonus muksun, Coregonus ussuriensis, Coregonus peled, Coregonus steinmanni, Coregonus albellus, Coregonus autumnalis, Stenodus leucichthys</t>
+  </si>
+  <si>
+    <t>Melanogrammus aeglefinus</t>
+  </si>
+  <si>
+    <t>100 matches: Gadus macrocephalus, Gadus morhua, Gadus chalcogrammus</t>
+  </si>
+  <si>
+    <t>no 100% match: 95.57 Delphinapterus leucas, Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.19% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>no 100% match (no matches that make sense) - likely Mammalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no 100% match: 98.08% Erignathus barbatus </t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36 Sus scrofa</t>
+  </si>
+  <si>
+    <t>No 100% match: 99.37% Coregonus nasus</t>
+  </si>
+  <si>
+    <t>No 100% match: 99.08% Gymnocanthus tricuspis, Gymnocanthus intermedius, Gymnocanthus pistilliger</t>
+  </si>
+  <si>
+    <t>No 100% match: 94.90% Gymnocanthus tricuspis, Gymnocanthus intermedius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% matches: Myoxocephalus quadricornis, Myoxocephalus aenaeus, Myoxocephalus scorpius, Myoxocephalus thompsonii </t>
+  </si>
+  <si>
+    <t>no 100% matches -  CHECK IF MAMMALIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No 100% match: 99.05% Clupea harengus, Clupea pallasii, Sprattus sprattus, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% matches: Myzopsetta proboscidea, Glyptocephalus zachirus, Glyptocephalus stelleri, </t>
+  </si>
+  <si>
+    <t>No 100% match: 97.94% Osmerus mordax dentex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% matches: "Uncultured bacterium," Bisgaardia miroungae, Bisgaardia hudsonensis, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no 100% match: 99.36% Thunnus alalunga, Thunnus thynnus, Thunnus orientalis, </t>
+  </si>
+  <si>
+    <t>no 100% match (no match that made sense)</t>
+  </si>
+  <si>
+    <t>No 100% match: 98.10% Sagmatias obliquidens - MAMMALIA</t>
+  </si>
+  <si>
+    <t>100% matches: Ammodytes tobianus, Ammodytes personatus, Hyperoplus lanceolatus, Hyperoplus immaculatus, Ammodytes japonicus, Ammodytes marinus, Ammodytes hexapterus</t>
+  </si>
+  <si>
+    <t>100% matches: Glyptocephalus zachirus, Platichthys stellatus, Kareius bicoloratus x Platichthys stellatus (hybrid), Hippoglossus stenolepis, Limanda limanda, Limanda sakhalinensis, Hippoglossus hippoglossus , Hippoglossoides robustus, Platichthys flesus, Hippoglossoides elassodon, Myzopsetta ferruginea, Platichthys stellatus x Verasper variegatus (hybrid), Hippoglossoides dubius, Limanda aspera, Liopsetta glacialis , Hippoglossoides platessoides, Cleisthenes pinetorum, Myzopsetta proboscidea, Cleisthenes herzensteini, Glyptocephalus zachirus</t>
+  </si>
+  <si>
+    <t>100% matches: "Uncultured bacterium," Clostridium sporogenes, Clostridium niameyense</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% matches: "Uncultured bacterium," "Uncultured Clostridium" </t>
+  </si>
+  <si>
+    <t>no 100% match: 91.14% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>Lumpenus sagitta</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.05% Delphinapterus leucas, Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 91.14% Delphinapterus leucas, Monodon monoceros</t>
+  </si>
+  <si>
+    <t>no 100% match: 98.73% Cottus cognatus</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.44% Eleginus gracilis</t>
+  </si>
+  <si>
+    <t>100% matches: Sebastes mystinus, Sebastes entomelas</t>
+  </si>
+  <si>
+    <t>no 100% matches: 89.74% Delphinapterus leucas</t>
+  </si>
+  <si>
+    <t>&lt;- SOMEWHAT QUESTIONABLE, BASED ON THEIR ATLANTIC DISTRIBUTION</t>
+  </si>
+  <si>
+    <t>100% matches: Platichthys stellatus, Myzopsetta ferruginea, Platichthys flesus, Liopsetta glacialis, Kareius bicoloratus x Platichthys stellatus (a hybrid), Platichthys stellatus x Verasper variegatus (a hybrid)</t>
+  </si>
+  <si>
+    <t>100% matches: Hippoglossoides robustus, Limanda limanda, Limanda aspera, Hippoglossoides elassodon, Limanda sakhalinensis, Hippoglossoides platessoides, Hippoglossoides dubius, Cleisthenes pinetorum, Cleisthenes herzensteini</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Myoxocephalus quadricornis, Myoxocephalus aenaeus, Myoxocephalus scorpius, Myoxocephalus thompsonii</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.36% Platichthys stellatus, Kareius bicoloratus x Platichthys stellatus (hybrid), Platichthys flesus, Myzopsetta ferruginea, Platichthys stellatus x Verasper variegatus (hybrid), Liopsetta glacialis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1216,13 +1559,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF212121"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1235,6 +1585,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1245,18 +1605,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1273,9 +1639,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1313,9 +1679,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1350,7 +1716,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1385,7 +1751,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1558,26 +1924,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I290"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="I283" sqref="I283"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1606,7 +1972,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1632,30 +1998,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="5" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1681,7 +2047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1707,7 +2073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -1730,7 +2096,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1756,7 +2122,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1782,7 +2148,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1808,7 +2174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1831,7 +2197,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1857,7 +2223,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1883,30 +2249,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="5" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1932,24 +2298,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1972,7 +2338,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1995,7 +2361,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2014,8 +2380,11 @@
       <c r="F18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2034,8 +2403,11 @@
       <c r="F19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2061,7 +2433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -2077,8 +2449,11 @@
       <c r="E21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -2097,8 +2472,11 @@
       <c r="F22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -2120,8 +2498,11 @@
       <c r="G23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2140,25 +2521,31 @@
       <c r="F24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="I24" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="B25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I25" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2177,8 +2564,11 @@
       <c r="F26" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I26" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -2197,8 +2587,11 @@
       <c r="F27" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I27" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2217,8 +2610,11 @@
       <c r="F28" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I28" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -2244,7 +2640,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2263,8 +2659,11 @@
       <c r="F30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2290,7 +2689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -2316,7 +2715,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2335,8 +2734,11 @@
       <c r="F33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -2358,28 +2760,34 @@
       <c r="G34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="I34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="B35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2398,8 +2806,11 @@
       <c r="F36" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -2425,7 +2836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -2447,8 +2858,11 @@
       <c r="G38" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2470,8 +2884,11 @@
       <c r="G39" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2490,8 +2907,11 @@
       <c r="F40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2517,7 +2937,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -2543,27 +2963,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="B43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2582,8 +3005,11 @@
       <c r="F44" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2602,8 +3028,11 @@
       <c r="F45" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2622,8 +3051,11 @@
       <c r="F46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I46" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2642,8 +3074,11 @@
       <c r="F47" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I47" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2662,8 +3097,11 @@
       <c r="F48" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -2689,7 +3127,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2708,8 +3146,11 @@
       <c r="F50" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -2735,7 +3176,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -2761,7 +3202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2780,8 +3221,11 @@
       <c r="F53" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -2807,7 +3251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2826,8 +3270,11 @@
       <c r="F55" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2843,8 +3290,11 @@
       <c r="E56" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>105</v>
       </c>
@@ -2863,8 +3313,11 @@
       <c r="F57" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -2890,7 +3343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>107</v>
       </c>
@@ -2916,7 +3369,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>108</v>
       </c>
@@ -2942,7 +3395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>109</v>
       </c>
@@ -2968,7 +3421,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>110</v>
       </c>
@@ -2994,7 +3447,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>111</v>
       </c>
@@ -3013,8 +3466,11 @@
       <c r="F63" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>112</v>
       </c>
@@ -3040,7 +3496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>113</v>
       </c>
@@ -3066,7 +3522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>114</v>
       </c>
@@ -3085,8 +3541,11 @@
       <c r="F66" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I66" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>115</v>
       </c>
@@ -3112,27 +3571,30 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="68" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" t="s">
-        <v>17</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="B68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I68" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>117</v>
       </c>
@@ -3151,28 +3613,34 @@
       <c r="F69" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+      <c r="I69" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B70" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" t="s">
-        <v>17</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="B70" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I70" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>119</v>
       </c>
@@ -3191,8 +3659,11 @@
       <c r="F71" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I71" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>120</v>
       </c>
@@ -3218,7 +3689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>121</v>
       </c>
@@ -3244,7 +3715,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -3270,7 +3741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>123</v>
       </c>
@@ -3289,8 +3760,11 @@
       <c r="F75" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I75" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>124</v>
       </c>
@@ -3306,8 +3780,11 @@
       <c r="E76" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I76" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>125</v>
       </c>
@@ -3326,8 +3803,11 @@
       <c r="F77" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I77" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>126</v>
       </c>
@@ -3353,7 +3833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>127</v>
       </c>
@@ -3372,8 +3852,11 @@
       <c r="F79" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I79" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>128</v>
       </c>
@@ -3392,8 +3875,11 @@
       <c r="F80" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>129</v>
       </c>
@@ -3419,7 +3905,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>130</v>
       </c>
@@ -3438,8 +3924,11 @@
       <c r="F82" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I82" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>131</v>
       </c>
@@ -3465,7 +3954,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>132</v>
       </c>
@@ -3484,8 +3973,11 @@
       <c r="F84" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I84" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>133</v>
       </c>
@@ -3501,8 +3993,11 @@
       <c r="E85" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I85" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>134</v>
       </c>
@@ -3518,8 +4013,11 @@
       <c r="E86" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I86" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>135</v>
       </c>
@@ -3545,7 +4043,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>138</v>
       </c>
@@ -3564,8 +4062,11 @@
       <c r="F88" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>139</v>
       </c>
@@ -3584,45 +4085,54 @@
       <c r="F89" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+      <c r="I89" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B90" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90" t="s">
-        <v>10</v>
-      </c>
-      <c r="D90" t="s">
-        <v>17</v>
-      </c>
-      <c r="E90" t="s">
+      <c r="B90" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="I90" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B91" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" t="s">
-        <v>10</v>
-      </c>
-      <c r="D91" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" t="s">
+      <c r="B91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>142</v>
       </c>
@@ -3632,8 +4142,11 @@
       <c r="C92" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I92" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -3659,7 +4172,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>144</v>
       </c>
@@ -3685,7 +4198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>145</v>
       </c>
@@ -3704,8 +4217,11 @@
       <c r="F95" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>146</v>
       </c>
@@ -3731,7 +4247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>147</v>
       </c>
@@ -3750,8 +4266,11 @@
       <c r="F97" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I97" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>148</v>
       </c>
@@ -3770,8 +4289,11 @@
       <c r="F98" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I98" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>149</v>
       </c>
@@ -3790,8 +4312,11 @@
       <c r="F99" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I99" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>150</v>
       </c>
@@ -3817,7 +4342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>151</v>
       </c>
@@ -3836,8 +4361,11 @@
       <c r="F101" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I101" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>152</v>
       </c>
@@ -3863,7 +4391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>153</v>
       </c>
@@ -3889,7 +4417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>154</v>
       </c>
@@ -3899,8 +4427,11 @@
       <c r="C104" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I104" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>155</v>
       </c>
@@ -3926,27 +4457,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="106" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C106" t="s">
-        <v>10</v>
-      </c>
-      <c r="D106" t="s">
-        <v>17</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="B106" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E106" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F106" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I106" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>157</v>
       </c>
@@ -3965,25 +4499,31 @@
       <c r="F107" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+      <c r="I107" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B108" t="s">
-        <v>9</v>
-      </c>
-      <c r="C108" t="s">
-        <v>10</v>
-      </c>
-      <c r="D108" t="s">
-        <v>17</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="B108" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E108" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I108" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>159</v>
       </c>
@@ -4009,7 +4549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>160</v>
       </c>
@@ -4028,8 +4568,11 @@
       <c r="F110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I110" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>161</v>
       </c>
@@ -4045,8 +4588,11 @@
       <c r="E111" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I111" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>162</v>
       </c>
@@ -4072,7 +4618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>163</v>
       </c>
@@ -4091,8 +4637,11 @@
       <c r="F113" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I113" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>164</v>
       </c>
@@ -4118,7 +4667,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>165</v>
       </c>
@@ -4144,7 +4693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>166</v>
       </c>
@@ -4170,7 +4719,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>167</v>
       </c>
@@ -4196,7 +4745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>168</v>
       </c>
@@ -4215,8 +4764,11 @@
       <c r="F118" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I118" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>170</v>
       </c>
@@ -4235,8 +4787,11 @@
       <c r="F119" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I119" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>171</v>
       </c>
@@ -4262,7 +4817,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>172</v>
       </c>
@@ -4272,8 +4827,11 @@
       <c r="C121" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I121" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>173</v>
       </c>
@@ -4289,8 +4847,11 @@
       <c r="E122" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I122" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>174</v>
       </c>
@@ -4309,8 +4870,11 @@
       <c r="F123" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I123" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>175</v>
       </c>
@@ -4326,8 +4890,11 @@
       <c r="E124" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I124" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>176</v>
       </c>
@@ -4353,7 +4920,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>177</v>
       </c>
@@ -4379,7 +4946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>178</v>
       </c>
@@ -4398,8 +4965,11 @@
       <c r="F127" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I127" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>179</v>
       </c>
@@ -4425,7 +4995,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>180</v>
       </c>
@@ -4441,8 +5011,11 @@
       <c r="E129" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I129" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>181</v>
       </c>
@@ -4468,7 +5041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>182</v>
       </c>
@@ -4478,8 +5051,11 @@
       <c r="C131" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I131" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>183</v>
       </c>
@@ -4505,7 +5081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>184</v>
       </c>
@@ -4531,7 +5107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>185</v>
       </c>
@@ -4557,7 +5133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>186</v>
       </c>
@@ -4573,8 +5149,11 @@
       <c r="E135" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I135" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>187</v>
       </c>
@@ -4593,8 +5172,11 @@
       <c r="F136" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I136" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>188</v>
       </c>
@@ -4616,8 +5198,11 @@
       <c r="G137" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I137" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>189</v>
       </c>
@@ -4643,7 +5228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>190</v>
       </c>
@@ -4662,8 +5247,11 @@
       <c r="F139" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I139" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>191</v>
       </c>
@@ -4689,7 +5277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>192</v>
       </c>
@@ -4715,7 +5303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>193</v>
       </c>
@@ -4741,7 +5329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>194</v>
       </c>
@@ -4767,7 +5355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>195</v>
       </c>
@@ -4786,8 +5374,11 @@
       <c r="F144" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I144" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>196</v>
       </c>
@@ -4803,8 +5394,11 @@
       <c r="E145" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I145" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>197</v>
       </c>
@@ -4830,7 +5424,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>198</v>
       </c>
@@ -4849,8 +5443,11 @@
       <c r="F147" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I147" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>199</v>
       </c>
@@ -4876,7 +5473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>200</v>
       </c>
@@ -4892,8 +5489,11 @@
       <c r="E149" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I149" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>201</v>
       </c>
@@ -4919,7 +5519,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>202</v>
       </c>
@@ -4945,7 +5545,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>203</v>
       </c>
@@ -4961,8 +5561,11 @@
       <c r="E152" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I152" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>204</v>
       </c>
@@ -4981,8 +5584,11 @@
       <c r="F153" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I153" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>205</v>
       </c>
@@ -5001,8 +5607,11 @@
       <c r="F154" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I154" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>206</v>
       </c>
@@ -5021,8 +5630,11 @@
       <c r="F155" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I155" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>207</v>
       </c>
@@ -5048,7 +5660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>208</v>
       </c>
@@ -5074,7 +5686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>209</v>
       </c>
@@ -5093,8 +5705,11 @@
       <c r="F158" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I158" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>210</v>
       </c>
@@ -5120,7 +5735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>211</v>
       </c>
@@ -5139,8 +5754,11 @@
       <c r="F160" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I160" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>212</v>
       </c>
@@ -5166,7 +5784,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>215</v>
       </c>
@@ -5192,7 +5810,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>216</v>
       </c>
@@ -5214,8 +5832,11 @@
       <c r="G163" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I163" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>217</v>
       </c>
@@ -5238,7 +5859,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>218</v>
       </c>
@@ -5248,8 +5869,11 @@
       <c r="C165" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I165" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>219</v>
       </c>
@@ -5275,7 +5899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>220</v>
       </c>
@@ -5301,7 +5925,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>223</v>
       </c>
@@ -5327,7 +5951,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>228</v>
       </c>
@@ -5353,7 +5977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>229</v>
       </c>
@@ -5379,7 +6003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>230</v>
       </c>
@@ -5405,7 +6029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>231</v>
       </c>
@@ -5431,7 +6055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>232</v>
       </c>
@@ -5447,8 +6071,11 @@
       <c r="E173" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I173" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>233</v>
       </c>
@@ -5467,8 +6094,11 @@
       <c r="F174" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I174" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>234</v>
       </c>
@@ -5487,8 +6117,11 @@
       <c r="F175" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I175" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>235</v>
       </c>
@@ -5514,7 +6147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>236</v>
       </c>
@@ -5530,8 +6163,11 @@
       <c r="E177" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I177" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>237</v>
       </c>
@@ -5550,8 +6186,11 @@
       <c r="F178" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I178" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>238</v>
       </c>
@@ -5570,8 +6209,11 @@
       <c r="F179" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I179" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>239</v>
       </c>
@@ -5587,8 +6229,11 @@
       <c r="E180" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I180" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>240</v>
       </c>
@@ -5598,8 +6243,11 @@
       <c r="C181" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I181" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>241</v>
       </c>
@@ -5621,8 +6269,11 @@
       <c r="G182" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I182" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>242</v>
       </c>
@@ -5648,7 +6299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>243</v>
       </c>
@@ -5664,8 +6315,11 @@
       <c r="E184" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I184" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>244</v>
       </c>
@@ -5684,28 +6338,34 @@
       <c r="F185" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
+      <c r="I185" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B186" t="s">
-        <v>9</v>
-      </c>
-      <c r="C186" t="s">
-        <v>10</v>
-      </c>
-      <c r="D186" t="s">
-        <v>17</v>
-      </c>
-      <c r="E186" t="s">
+      <c r="B186" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C186" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D186" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E186" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F186" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I186" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>246</v>
       </c>
@@ -5721,8 +6381,11 @@
       <c r="E187" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I187" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>247</v>
       </c>
@@ -5738,8 +6401,11 @@
       <c r="E188" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I188" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>248</v>
       </c>
@@ -5758,28 +6424,34 @@
       <c r="F189" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
+      <c r="I189" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B190" t="s">
-        <v>9</v>
-      </c>
-      <c r="C190" t="s">
-        <v>10</v>
-      </c>
-      <c r="D190" t="s">
-        <v>17</v>
-      </c>
-      <c r="E190" t="s">
+      <c r="B190" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E190" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F190" t="s">
+      <c r="F190" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I190" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>250</v>
       </c>
@@ -5795,8 +6467,11 @@
       <c r="E191" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I191" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>251</v>
       </c>
@@ -5806,31 +6481,37 @@
       <c r="C192" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
+      <c r="I192" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B193" t="s">
-        <v>9</v>
-      </c>
-      <c r="C193" t="s">
-        <v>10</v>
-      </c>
-      <c r="D193" t="s">
-        <v>17</v>
-      </c>
-      <c r="E193" t="s">
+      <c r="B193" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E193" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F193" t="s">
+      <c r="F193" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G193" t="s">
+      <c r="G193" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I193" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>253</v>
       </c>
@@ -5843,8 +6524,11 @@
       <c r="D194" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I194" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>254</v>
       </c>
@@ -5866,8 +6550,11 @@
       <c r="G195" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I195" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>255</v>
       </c>
@@ -5877,8 +6564,11 @@
       <c r="C196" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I196" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>256</v>
       </c>
@@ -5891,8 +6581,11 @@
       <c r="D197" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I197" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>257</v>
       </c>
@@ -5914,8 +6607,11 @@
       <c r="G198" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I198" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>258</v>
       </c>
@@ -5931,8 +6627,11 @@
       <c r="E199" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I199" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>259</v>
       </c>
@@ -5958,7 +6657,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>260</v>
       </c>
@@ -5984,7 +6683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>261</v>
       </c>
@@ -6010,7 +6709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>262</v>
       </c>
@@ -6029,8 +6728,11 @@
       <c r="F203" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I203" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>263</v>
       </c>
@@ -6040,8 +6742,11 @@
       <c r="C204" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I204" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>264</v>
       </c>
@@ -6057,8 +6762,11 @@
       <c r="E205" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I205" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>265</v>
       </c>
@@ -6077,8 +6785,11 @@
       <c r="F206" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I206" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>266</v>
       </c>
@@ -6104,7 +6815,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>270</v>
       </c>
@@ -6120,8 +6831,11 @@
       <c r="E208" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I208" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>271</v>
       </c>
@@ -6147,7 +6861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>272</v>
       </c>
@@ -6166,8 +6880,11 @@
       <c r="F210" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I210" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>273</v>
       </c>
@@ -6183,8 +6900,11 @@
       <c r="E211" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I211" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>274</v>
       </c>
@@ -6203,8 +6923,11 @@
       <c r="F212" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I212" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>275</v>
       </c>
@@ -6220,8 +6943,11 @@
       <c r="E213" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I213" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>276</v>
       </c>
@@ -6231,8 +6957,11 @@
       <c r="C214" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I214" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>277</v>
       </c>
@@ -6242,28 +6971,34 @@
       <c r="C215" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
+      <c r="I215" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B216" t="s">
-        <v>9</v>
-      </c>
-      <c r="C216" t="s">
-        <v>10</v>
-      </c>
-      <c r="D216" t="s">
-        <v>17</v>
-      </c>
-      <c r="E216" t="s">
+      <c r="B216" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D216" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E216" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F216" t="s">
+      <c r="F216" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I216" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>279</v>
       </c>
@@ -6289,7 +7024,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>280</v>
       </c>
@@ -6308,8 +7043,11 @@
       <c r="F218" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I218" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>281</v>
       </c>
@@ -6335,27 +7073,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
+    <row r="220" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B220" t="s">
-        <v>9</v>
-      </c>
-      <c r="C220" t="s">
-        <v>10</v>
-      </c>
-      <c r="D220" t="s">
-        <v>17</v>
-      </c>
-      <c r="E220" t="s">
+      <c r="B220" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D220" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E220" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F220" t="s">
+      <c r="F220" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I220" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>283</v>
       </c>
@@ -6374,8 +7115,11 @@
       <c r="F221" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I221" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>284</v>
       </c>
@@ -6391,8 +7135,11 @@
       <c r="E222" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I222" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>285</v>
       </c>
@@ -6418,7 +7165,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>290</v>
       </c>
@@ -6434,8 +7181,11 @@
       <c r="E224" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I224" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>291</v>
       </c>
@@ -6454,8 +7204,11 @@
       <c r="F225" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I225" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>292</v>
       </c>
@@ -6481,7 +7234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>293</v>
       </c>
@@ -6507,7 +7260,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>296</v>
       </c>
@@ -6517,8 +7270,11 @@
       <c r="C228" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I228" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>297</v>
       </c>
@@ -6534,8 +7290,11 @@
       <c r="E229" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I229" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>298</v>
       </c>
@@ -6561,7 +7320,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>299</v>
       </c>
@@ -6577,8 +7336,11 @@
       <c r="E231" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I231" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>300</v>
       </c>
@@ -6588,8 +7350,11 @@
       <c r="C232" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I232" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>301</v>
       </c>
@@ -6605,8 +7370,11 @@
       <c r="E233" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I233" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>302</v>
       </c>
@@ -6622,28 +7390,34 @@
       <c r="E234" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A235" t="s">
+      <c r="I234" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B235" t="s">
-        <v>9</v>
-      </c>
-      <c r="C235" t="s">
-        <v>10</v>
-      </c>
-      <c r="D235" t="s">
-        <v>17</v>
-      </c>
-      <c r="E235" t="s">
+      <c r="B235" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E235" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F235" t="s">
+      <c r="F235" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I235" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>304</v>
       </c>
@@ -6669,7 +7443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>305</v>
       </c>
@@ -6685,8 +7459,11 @@
       <c r="E237" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I237" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>306</v>
       </c>
@@ -6702,19 +7479,28 @@
       <c r="E238" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
+      <c r="I238" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="B239" t="s">
-        <v>9</v>
-      </c>
-      <c r="C239" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B239" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I239" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="L239" s="5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>308</v>
       </c>
@@ -6736,8 +7522,11 @@
       <c r="G240" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I240" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>309</v>
       </c>
@@ -6753,8 +7542,11 @@
       <c r="E241" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I241" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>310</v>
       </c>
@@ -6770,8 +7562,11 @@
       <c r="E242" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I242" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>311</v>
       </c>
@@ -6781,8 +7576,11 @@
       <c r="C243" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I243" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>312</v>
       </c>
@@ -6801,8 +7599,11 @@
       <c r="F244" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I244" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>313</v>
       </c>
@@ -6824,8 +7625,11 @@
       <c r="G245" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I245" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>316</v>
       </c>
@@ -6835,8 +7639,11 @@
       <c r="C246" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I246" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>317</v>
       </c>
@@ -6862,7 +7669,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>320</v>
       </c>
@@ -6878,8 +7685,11 @@
       <c r="E248" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I248" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>321</v>
       </c>
@@ -6895,8 +7705,11 @@
       <c r="E249" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I249" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>322</v>
       </c>
@@ -6906,8 +7719,11 @@
       <c r="C250" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I250" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>323</v>
       </c>
@@ -6929,39 +7745,48 @@
       <c r="G251" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
+      <c r="I251" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="B252" t="s">
-        <v>9</v>
-      </c>
-      <c r="C252" t="s">
-        <v>10</v>
-      </c>
-      <c r="D252" t="s">
-        <v>17</v>
-      </c>
-      <c r="E252" t="s">
+      <c r="B252" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C252" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D252" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E252" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F252" t="s">
+      <c r="F252" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
+      <c r="I252" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B253" t="s">
-        <v>9</v>
-      </c>
-      <c r="C253" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B253" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C253" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I253" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>326</v>
       </c>
@@ -6987,7 +7812,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>328</v>
       </c>
@@ -6997,8 +7822,11 @@
       <c r="C255" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I255" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>329</v>
       </c>
@@ -7011,8 +7839,11 @@
       <c r="D256" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I256" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>330</v>
       </c>
@@ -7031,8 +7862,11 @@
       <c r="F257" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I257" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>331</v>
       </c>
@@ -7051,8 +7885,11 @@
       <c r="F258" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I258" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>332</v>
       </c>
@@ -7062,8 +7899,11 @@
       <c r="C259" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I259" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>333</v>
       </c>
@@ -7089,7 +7929,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>336</v>
       </c>
@@ -7102,8 +7942,11 @@
       <c r="D261" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I261" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>337</v>
       </c>
@@ -7129,7 +7972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>338</v>
       </c>
@@ -7139,8 +7982,11 @@
       <c r="C263" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I263" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>339</v>
       </c>
@@ -7166,7 +8012,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>343</v>
       </c>
@@ -7182,8 +8028,11 @@
       <c r="E265" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I265" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>345</v>
       </c>
@@ -7199,8 +8048,11 @@
       <c r="E266" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I266" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>346</v>
       </c>
@@ -7226,7 +8078,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>350</v>
       </c>
@@ -7252,7 +8104,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>353</v>
       </c>
@@ -7278,7 +8130,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>356</v>
       </c>
@@ -7288,8 +8140,11 @@
       <c r="C270" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I270" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>357</v>
       </c>
@@ -7315,7 +8170,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>358</v>
       </c>
@@ -7341,7 +8196,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>359</v>
       </c>
@@ -7360,8 +8215,11 @@
       <c r="F273" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I273" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>360</v>
       </c>
@@ -7374,8 +8232,11 @@
       <c r="D274" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I274" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>361</v>
       </c>
@@ -7394,8 +8255,11 @@
       <c r="F275" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I275" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>362</v>
       </c>
@@ -7405,8 +8269,11 @@
       <c r="C276" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I276" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>363</v>
       </c>
@@ -7416,8 +8283,14 @@
       <c r="C277" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H277" t="s">
+        <v>490</v>
+      </c>
+      <c r="I277" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>364</v>
       </c>
@@ -7443,7 +8316,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>369</v>
       </c>
@@ -7459,28 +8332,34 @@
       <c r="E279" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A280" t="s">
+      <c r="I279" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="B280" t="s">
-        <v>9</v>
-      </c>
-      <c r="C280" t="s">
-        <v>10</v>
-      </c>
-      <c r="D280" t="s">
-        <v>17</v>
-      </c>
-      <c r="E280" t="s">
+      <c r="B280" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C280" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D280" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E280" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F280" t="s">
+      <c r="F280" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I280" s="5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>371</v>
       </c>
@@ -7490,8 +8369,11 @@
       <c r="C281" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I281" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>372</v>
       </c>
@@ -7507,8 +8389,11 @@
       <c r="E282" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I282" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>373</v>
       </c>
@@ -7527,8 +8412,11 @@
       <c r="F283" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I283" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>374</v>
       </c>
@@ -7547,8 +8435,11 @@
       <c r="F284" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I284" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>375</v>
       </c>
@@ -7570,8 +8461,11 @@
       <c r="G285" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I285" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>378</v>
       </c>
@@ -7597,7 +8491,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>379</v>
       </c>
@@ -7613,8 +8507,11 @@
       <c r="E287" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I287" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>380</v>
       </c>
@@ -7633,8 +8530,11 @@
       <c r="F288" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I288" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>381</v>
       </c>
@@ -7660,7 +8560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>382</v>
       </c>

</xml_diff>

<commit_message>
Update 12S and 16S to most recent tax reference
</commit_message>
<xml_diff>
--- a/DADA2/WADE003-arcticpred-12SP1-taxa-130trunc.xlsx
+++ b/DADA2/WADE003-arcticpred-12SP1-taxa-130trunc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\DADA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B3A1E5-D211-4015-BBBB-78A9FC9975E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23D0509-919F-45AE-BC5A-013443C70812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1964,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A295" sqref="A295"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J1" activeCellId="1" sqref="I1:I1048576 J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>